<commit_message>
Merged PR 16: merge demo_hello_world to master
Related work items: #194, #40
</commit_message>
<xml_diff>
--- a/DesignerRawdata/Excel/Chapter1.xlsx
+++ b/DesignerRawdata/Excel/Chapter1.xlsx
@@ -3,17 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{63C59682-3597-4E87-A940-A57D00E118C5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{16EFE39C-0CB9-447E-A7CB-CD004C9FC1A9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter1-1" sheetId="1" r:id="rId1"/>
     <sheet name="Chapter1-2" sheetId="4" r:id="rId2"/>
-    <sheet name="ChapterTest" sheetId="5" r:id="rId3"/>
+    <sheet name="Chapter1-2_Choice" sheetId="6" r:id="rId3"/>
+    <sheet name="ChapterTest" sheetId="5" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="DialogueTalkerName.xlsx">[1]!DialogueTalkerNameID</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="63">
   <si>
     <t>id_chapter_title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,6 +43,60 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>DialogueText</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DialogueTalkerNameID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_programmer</t>
+  </si>
+  <si>
+    <t>測試：Widget</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工程師</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>企畫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>美術</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>這個遊戲主要會展示 HorizonDialogue Plugin 內的一些主要的功能。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>話不多說，馬上讓我們來看看這個Plugin能夠做到那些事吧！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>choice000_00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>choice000_01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>choice000_02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_designer</t>
+  </si>
+  <si>
     <t>id_003</t>
   </si>
   <si>
@@ -51,54 +106,157 @@
     <t>id_005</t>
   </si>
   <si>
-    <t>Hello! 有人在嗎？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>你是來學</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DialogueText</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DialogueTalkerNameID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_programmer</t>
-  </si>
-  <si>
-    <t>第一種是CreateEventDialogueMsg，擁有比較少的參數需求。這個事件會試著將文字顯示在設置於DialogueScene.中的「DefaultDialogueMsgTextBlockWidgetName」。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>這個教學會展示如何將 DialogueEvent 加到 HorizonDialogueScene 中。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>測試：Widget</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>這個demo專案會展示 HorizonDialogue Plugin 內的一些主要的功能。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>話不多說，馬上讓我們開始本篇的教學吧！</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>當遊戲程式遇上遊戲美術</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_programmer</t>
+    <t>id_006</t>
+  </si>
+  <si>
+    <t>恩？有什麼事嗎？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_007</t>
+  </si>
+  <si>
+    <t>id_008</t>
+  </si>
+  <si>
+    <t>id_009</t>
+  </si>
+  <si>
+    <t>id_010</t>
+  </si>
+  <si>
+    <t>id_011</t>
+  </si>
+  <si>
+    <t>id_012</t>
+  </si>
+  <si>
+    <t>id_013</t>
+  </si>
+  <si>
+    <t>id_014</t>
+  </si>
+  <si>
+    <t>id_015</t>
+  </si>
+  <si>
+    <t>id_016</t>
+  </si>
+  <si>
+    <t>id_017</t>
+  </si>
+  <si>
+    <t>id_018</t>
+  </si>
+  <si>
+    <t>id_019</t>
+  </si>
+  <si>
+    <t>id_020</t>
+  </si>
+  <si>
+    <t>id_021</t>
+  </si>
+  <si>
+    <t>id_022</t>
+  </si>
+  <si>
+    <t>id_023</t>
+  </si>
+  <si>
+    <t>Hello！有人在嗎？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是想問這個Horizon Dialogue Plugin該怎麼使用嗎？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>聽起來蠻酷炫的，實際上是怎麼運作的呢？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一章：Horizon Dialogue Plugin簡介</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你想要從那邊開始了解起呢？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>簡單來說，這個Plugin的主要目標是想要建立一套遊戲系統框架。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>嗯，大致上有那麼一點感覺了。所以說HorizonUI的用途主要是用來顯示對話的囉？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>那HorizonTween呢？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是程式大大！正好有個問題想請教你？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以先談談Plugin主要的用途是什麼嗎？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>真不愧是大大！馬上就猜出我想問什麼了！剛剛才拿到這個Plugin，正困擾著該怎麼使用呢。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在套用這套系統框架之後，遊戲開發者就能夠隨意的在遊戲中加入各種對話演出與劇情。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首先，在開始使用這套Plugin之前，我建議先去研究HorizonUI、HorizonTween以及HorizonFramework這幾個Plugin的功能該怎麼使用。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是的，藉由HorizonUI中所提供的功能，就能夠實現多樣的文字對話效果。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>因為Dialogue Plugin非常緊密的整合了這幾套Plugin，並在增加了對話演出所需要的流程與功能。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>剛剛所提到的遊戲系統框架，跟HorizonFramework有什麼關係嗎？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是的，HorizonDialogue Plugin的系統框架就是對HorizonFramework進行擴增，二套Plugin在工作流程的設計基本上是一致的。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>只是為了加入對話事件，因此在HorizonScene的生命週期中新插入了：AddDialogueEvent這個事件。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HorizonTween的話，主要是拿來實現一些文字與圖片的動畫效果。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>例如：文字或圖片的移動、旋轉，或者是淡出跟淡入。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>好像有點複雜，有什麼快速入門的方法呢？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我想，先到GitHub上把這個專案Demo抓下來玩玩是最快的方法了。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在這之後我會示範幾個Plugin的進階用法。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>真令人期待！</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -185,6 +343,11 @@
         <row r="4">
           <cell r="A4" t="str">
             <v>id_artist</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>id_unknwon</v>
           </cell>
         </row>
       </sheetData>
@@ -459,7 +622,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -472,26 +635,26 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -509,26 +672,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="81" customWidth="1"/>
+    <col min="3" max="3" width="103.85546875" customWidth="1"/>
     <col min="4" max="4" width="27.42578125" customWidth="1"/>
     <col min="5" max="5" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -536,71 +699,280 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>DialogueTalkerName.xlsx</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -608,11 +980,61 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B349367-CC38-46D3-9977-E9F7CC21194C}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="41" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317EB572-536C-4780-970D-6CD10E8E263E}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -624,10 +1046,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -635,7 +1057,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -643,7 +1065,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -651,7 +1073,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged PR 17: demo_1-2
Related work items: #99
</commit_message>
<xml_diff>
--- a/DesignerRawdata/Excel/Chapter1.xlsx
+++ b/DesignerRawdata/Excel/Chapter1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{16EFE39C-0CB9-447E-A7CB-CD004C9FC1A9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{08F96577-ACD9-455A-89B9-2212A3692742}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -168,78 +168,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是想問這個Horizon Dialogue Plugin該怎麼使用嗎？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>聽起來蠻酷炫的，實際上是怎麼運作的呢？</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>第一章：Horizon Dialogue Plugin簡介</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>你想要從那邊開始了解起呢？</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>簡單來說，這個Plugin的主要目標是想要建立一套遊戲系統框架。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>嗯，大致上有那麼一點感覺了。所以說HorizonUI的用途主要是用來顯示對話的囉？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>那HorizonTween呢？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是程式大大！正好有個問題想請教你？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>可以先談談Plugin主要的用途是什麼嗎？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>真不愧是大大！馬上就猜出我想問什麼了！剛剛才拿到這個Plugin，正困擾著該怎麼使用呢。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>在套用這套系統框架之後，遊戲開發者就能夠隨意的在遊戲中加入各種對話演出與劇情。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>首先，在開始使用這套Plugin之前，我建議先去研究HorizonUI、HorizonTween以及HorizonFramework這幾個Plugin的功能該怎麼使用。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是的，藉由HorizonUI中所提供的功能，就能夠實現多樣的文字對話效果。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>因為Dialogue Plugin非常緊密的整合了這幾套Plugin，並在增加了對話演出所需要的流程與功能。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>剛剛所提到的遊戲系統框架，跟HorizonFramework有什麼關係嗎？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是的，HorizonDialogue Plugin的系統框架就是對HorizonFramework進行擴增，二套Plugin在工作流程的設計基本上是一致的。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>只是為了加入對話事件，因此在HorizonScene的生命週期中新插入了：AddDialogueEvent這個事件。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HorizonTween的話，主要是拿來實現一些文字與圖片的動畫效果。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>例如：文字或圖片的移動、旋轉，或者是淡出跟淡入。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -248,15 +188,75 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>我想，先到GitHub上把這個專案Demo抓下來玩玩是最快的方法了。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在這之後我會示範幾個Plugin的進階用法。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>真令人期待！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是程式大大！正好有個問題想請教你。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一章： Horizon Dialogue Plugin 簡介</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是想問這個 Horizon Dialogue Plugin 該怎麼使用嗎？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>真不愧是大大！馬上就猜出我想問什麼了！剛剛才拿到這個 Plugin ，正困擾著該怎麼使用呢。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以先談談 Plugin 主要的用途是什麼嗎？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>簡單來說，這個 Plugin 的主要目標是想要建立一套遊戲系統框架。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首先，在開始使用這套 Plugin 之前，我建議先去研究 HorizonUI 、 HorizonTween 以及 HorizonFramework 這幾個 Plugin 的功能該怎麼使用。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>因為 Dialogue Plugin 非常緊密的整合了這幾套 Plugin ，並在增加了對話演出所需要的流程與功能。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>剛剛所提到的遊戲系統框架，跟 HorizonFramework 有什麼關係嗎？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是的， HorizonDialogue Plugin 的系統框架就是對 HorizonFramework 進行擴增，二套 Plugin 在工作流程的設計基本上是一致的。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>只是為了加入對話事件，因此在 HorizonScene 的生命週期中新插入了： AddDialogueEvent 這個事件。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>嗯，大致上有那麼一點感覺了。所以說 HorizonUI 的用途主要是用來顯示對話的囉？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是的，藉由 HorizonUI 中所提供的功能，就能夠實現多樣的文字對話效果。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>那 HorizonTween 呢？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HorizonTween 的話，主要是拿來實現一些文字與圖片的動畫效果。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我想，先到 GitHub 上把這個專案 Demo 抓下來玩玩是最快的方法了。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在這之後我會示範幾個 Plugin 的進階用法。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -675,7 +675,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -699,7 +699,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -732,7 +732,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -743,7 +743,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -765,7 +765,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -776,7 +776,7 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -787,7 +787,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -798,7 +798,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -809,7 +809,7 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -820,7 +820,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -875,7 +875,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -886,7 +886,7 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -897,7 +897,7 @@
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -908,7 +908,7 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -919,7 +919,7 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -930,7 +930,7 @@
         <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -941,7 +941,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -952,7 +952,7 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -963,7 +963,7 @@
         <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjust widget folder position
</commit_message>
<xml_diff>
--- a/DesignerRawdata/Excel/Chapter1.xlsx
+++ b/DesignerRawdata/Excel/Chapter1.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{08F96577-ACD9-455A-89B9-2212A3692742}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{982C727B-9EBB-4A46-816B-0CBBFD9D6A67}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter1-1" sheetId="1" r:id="rId1"/>
     <sheet name="Chapter1-2" sheetId="4" r:id="rId2"/>
-    <sheet name="Chapter1-2_Choice" sheetId="6" r:id="rId3"/>
-    <sheet name="ChapterTest" sheetId="5" r:id="rId4"/>
+    <sheet name="Chapter1-3" sheetId="8" r:id="rId3"/>
+    <sheet name="Chapter1-3_Choice" sheetId="6" r:id="rId4"/>
+    <sheet name="ChapterTest" sheetId="5" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="DialogueTalkerName.xlsx">[1]!DialogueTalkerNameID</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="71">
   <si>
     <t>id_chapter_title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -58,18 +59,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>工程師</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>企畫</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>美術</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>這個遊戲主要會展示 HorizonDialogue Plugin 內的一些主要的功能。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -82,18 +71,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>choice000_00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>choice000_01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>choice000_02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>id_designer</t>
   </si>
   <si>
@@ -196,10 +173,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>第一章： Horizon Dialogue Plugin 簡介</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>是想問這個 Horizon Dialogue Plugin 該怎麼使用嗎？</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -257,6 +230,65 @@
   </si>
   <si>
     <t>在這之後我會示範幾個 Plugin 的進階用法。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Horizon Dialogue Plugin 簡介</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_artist</t>
+  </si>
+  <si>
+    <t>夕陽西下，街道上開始湧現下班的人潮，然而，horizon-studio的一天才正要開始。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>為了要趕上月底的遊戲展，全體員工已經連續加班超過了一個月，因此團隊中的成員也開始出現了不平的聲音。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>今天，我一定要求加薪！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>那麼，接下來該往哪走呢？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>choice_front_room</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前面的房間</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>choice_left_room</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>左邊的房間</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>choice_right_room</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>右邊的房間</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>choice_back_room</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>後面的房間</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首先發難的是團隊中的美術，今天的她下定決心要找出老闆，為自己平時的辛勞爭取金錢上的補償。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -643,10 +675,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -654,7 +686,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -674,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -699,18 +731,18 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -721,7 +753,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -729,241 +761,241 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -980,11 +1012,194 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA70356-5547-4602-9DB2-292607A0A437}">
+  <dimension ref="A1:C26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="103.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{63460F4F-E029-4182-93EF-0AB56927B2F6}">
+      <formula1>DialogueTalkerName.xlsx</formula1>
+    </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{11AFAEC2-B27B-4F28-A942-69D8C5A979E4}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B349367-CC38-46D3-9977-E9F7CC21194C}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1000,26 +1215,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1029,7 +1252,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317EB572-536C-4780-970D-6CD10E8E263E}">
   <dimension ref="A1:C4"/>
   <sheetViews>

</xml_diff>

<commit_message>
Merged PR 20: demo_choice to master
Related work items: #222, #223, #224, #225, #226, #241, #242, #249, #89
</commit_message>
<xml_diff>
--- a/DesignerRawdata/Excel/Chapter1.xlsx
+++ b/DesignerRawdata/Excel/Chapter1.xlsx
@@ -3,19 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{982C727B-9EBB-4A46-816B-0CBBFD9D6A67}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C57FB633-4D32-4CB7-B24F-6830AD72986B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter1-1" sheetId="1" r:id="rId1"/>
     <sheet name="Chapter1-2" sheetId="4" r:id="rId2"/>
-    <sheet name="Chapter1-3" sheetId="8" r:id="rId3"/>
-    <sheet name="Chapter1-3_Choice" sheetId="6" r:id="rId4"/>
-    <sheet name="ChapterTest" sheetId="5" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
     <definedName name="DialogueTalkerName.xlsx">[1]!DialogueTalkerNameID</definedName>
@@ -30,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
   <si>
     <t>id_chapter_title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,10 +52,6 @@
     <t>id_programmer</t>
   </si>
   <si>
-    <t>測試：Widget</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>這個遊戲主要會展示 HorizonDialogue Plugin 內的一些主要的功能。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -234,61 +227,6 @@
   </si>
   <si>
     <t>Horizon Dialogue Plugin 簡介</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_artist</t>
-  </si>
-  <si>
-    <t>夕陽西下，街道上開始湧現下班的人潮，然而，horizon-studio的一天才正要開始。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>為了要趕上月底的遊戲展，全體員工已經連續加班超過了一個月，因此團隊中的成員也開始出現了不平的聲音。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>今天，我一定要求加薪！</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>那麼，接下來該往哪走呢？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>choice_front_room</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>前面的房間</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>choice_left_room</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>左邊的房間</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>choice_right_room</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>右邊的房間</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>choice_back_room</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>後面的房間</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>首先發難的是團隊中的美術，今天的她下定決心要找出老闆，為自己平時的辛勞爭取金錢上的補償。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -675,10 +613,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -686,7 +624,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -706,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -731,18 +669,18 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -753,7 +691,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -761,241 +699,241 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1009,308 +947,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA70356-5547-4602-9DB2-292607A0A437}">
-  <dimension ref="A1:C26"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="103.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{63460F4F-E029-4182-93EF-0AB56927B2F6}">
-      <formula1>DialogueTalkerName.xlsx</formula1>
-    </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{11AFAEC2-B27B-4F28-A942-69D8C5A979E4}"/>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B349367-CC38-46D3-9977-E9F7CC21194C}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="41" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317EB572-536C-4780-970D-6CD10E8E263E}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="3">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{EC67CF3D-B42A-4B63-B11C-80044B4B83DA}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B1048576" xr:uid="{DD34395F-5721-472A-9ED8-C0E8699D2458}">
-      <formula1>DialogueTalkerName.xlsx</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{D6783A7B-4EC4-4EBC-84C8-B7DDBF146F29}">
-      <formula1>DialogueTalkerName.xlsx</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>